<commit_message>
Expression Engine Added, used for display rule
</commit_message>
<xml_diff>
--- a/kidase-presentation/samples/Kidase Presentation Template.xlsx
+++ b/kidase-presentation/samples/Kidase Presentation Template.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="116">
   <si>
     <t>LineId</t>
   </si>
@@ -72,6 +72,9 @@
     <t>LayoutOverride</t>
   </si>
   <si>
+    <t>DisplayRule</t>
+  </si>
+  <si>
     <t>ይ፡ካ</t>
   </si>
   <si>
@@ -114,6 +117,36 @@
     <t>Amen</t>
   </si>
   <si>
+    <t>እምነ በሐ፣ ቅድስት ቤተክርስቲያን፣ ሥርጉት አረፋቲሃ በዕንቍ ጳዝዮን፤እምነ በሐ፣ ቅድስት ቤተክርስቲያን።</t>
+  </si>
+  <si>
+    <t>ሰላም ላንቺ ይሁን፤ እናታችን ክብርት ቤተክርስቲያን። ግድግዳዎችሽ በጳዝዮን እንቍ የተጌጡ ናቸው፤ሰላም ላንቺ ይሁን! እናታችን ክብርት ቤተክርስቲያን።</t>
+  </si>
+  <si>
+    <t>ሰላም ነዓኺ ይኹን ኣዴና ቅድስት ቤተ ክርስቲያን፡ መናድቕኪ ብዕንቊ ጳዝዮን ዝተሠርገወ፡ ሰላም ነዓኺ ይኹን ኣዴና ቅድስት ቤተ ክርስቲያን።</t>
+  </si>
+  <si>
+    <t>Peace be unto you, our mother, O honorable church. Thy walls are embroidered with Topaz. Peace be unto, our mother, O honorable church</t>
+  </si>
+  <si>
+    <t>{"meta.dayOfWeek": {"$in": ["Mon","Tue","Thu"]}}</t>
+  </si>
+  <si>
+    <t>መስቀል አብርሃ! በከዋክብት አሠርገወ ሰማየ፤ እምኩሉሰ ፀሐይ አርአየ።መስቀል አብርሃ! በከዋክብት አሠርገወ ሰማየ።</t>
+  </si>
+  <si>
+    <t>መስቀልን አበራ! በኮከቦች ሰማይን አስጌጠ። ከሁሉም ፀሐይን አሳየ።መስቀል አበራ። በኮከቦች ሰማይን አስጌጠ።</t>
+  </si>
+  <si>
+    <t>መስቀል ኣብርሀ፡ ብከዋኽብቲ ሰማይ ኣሠርገወ፡ ካብ ኩሉ ድማ ፀሓይ ኣርኣየ። መስቀል ኣብርሀ፡ ብከዋኽብቲ ሰማይ ኣሠርገወ።</t>
+  </si>
+  <si>
+    <t>The cross shined  and had the heavens embroidered with stars. Of all the sun is seen. The cross shined and had the heavens embroidered with stars.</t>
+  </si>
+  <si>
+    <t>{"meta.dayOfWeek": {"$in": ["Wed","Fri","Sat"]}}</t>
+  </si>
+  <si>
     <t>ኵሉ፡ ዘገብራ፡ ለጽድቅ፡ ጻድቀ፡ ውእቱ፡ ወዘያከብር፡ ሰንበተ። ኢይበል ፡ ፈላሲ፡ ዘገብአ፡ ኀበ፡ እግዚአብሔር፡</t>
   </si>
   <si>
@@ -124,6 +157,9 @@
   </si>
   <si>
     <t>Blessed is he who does blessed deeds and honors the Sabbath. Let him not question whether he will be outcast from the multitudes</t>
+  </si>
+  <si>
+    <t>{"meta.dayOfWeek": {"$in": ["Sun"]}}</t>
   </si>
   <si>
     <t>ይፈልጠኒኑ፡ እምሕዝቡ። ኵሉ፡ ዘገብራ፡ ለጽድቅ፡ ጻድቅ፡ ውእቱ፡ ወዘያከብር፡ ሰንበተ።</t>
@@ -608,7 +644,8 @@
     <col customWidth="1" min="9" max="9" width="41.29"/>
     <col customWidth="1" min="10" max="18" width="20.14"/>
     <col customWidth="1" min="19" max="19" width="14.29"/>
-    <col customWidth="1" min="20" max="34" width="8.71"/>
+    <col customWidth="1" min="20" max="20" width="49.14"/>
+    <col customWidth="1" min="21" max="34" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -669,528 +706,562 @@
       <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="T1" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="2">
       <c r="B2" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3">
       <c r="F3" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="5">
+      <c r="B5" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="F5" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="7">
       <c r="F7" s="2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9">
       <c r="F9" s="2" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" s="3" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11">
       <c r="F11" s="2" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12">
+      <c r="B12" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="F12" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="M12" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="F13" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="F14" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J14" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N12" s="2" t="s">
+      <c r="M14" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="2" t="s">
+      <c r="N14" s="2" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="B13" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="M13" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="N13" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="B14" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="M14" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="N14" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
       <c r="Q15" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
       <c r="Q16" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
       <c r="Q17" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
       <c r="Q18" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
       <c r="Q19" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
       <c r="Q20" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
       <c r="Q21" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
       <c r="Q22" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="M23" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="N23" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="24" ht="15.75" customHeight="1">
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-    </row>
-    <row r="25" ht="15.75" customHeight="1">
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="4"/>
+      <c r="Q23" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="M24" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="N24" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="O24" s="4"/>
+      <c r="P24" s="4"/>
+      <c r="Q24" s="2" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="F26" s="4"/>
@@ -6975,6 +7046,18 @@
       <c r="G989" s="4"/>
       <c r="H989" s="4"/>
       <c r="I989" s="4"/>
+    </row>
+    <row r="990" ht="15.75" customHeight="1">
+      <c r="F990" s="4"/>
+      <c r="G990" s="4"/>
+      <c r="H990" s="4"/>
+      <c r="I990" s="4"/>
+    </row>
+    <row r="991" ht="15.75" customHeight="1">
+      <c r="F991" s="4"/>
+      <c r="G991" s="4"/>
+      <c r="H991" s="4"/>
+      <c r="I991" s="4"/>
     </row>
   </sheetData>
   <printOptions/>
@@ -7003,48 +7086,48 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -8052,26 +8135,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Engine tested using ethiopian holiday
</commit_message>
<xml_diff>
--- a/kidase-presentation/samples/Kidase Presentation Template.xlsx
+++ b/kidase-presentation/samples/Kidase Presentation Template.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="121">
   <si>
     <t>LineId</t>
   </si>
@@ -208,6 +208,25 @@
   </si>
   <si>
     <t>and disdained to stand before the heavenly King, the King of Body and Spirit. This, the Apostles have taught us in their cannons.</t>
+  </si>
+  <si>
+    <t>ሃሌ ሉያ ዮሴፍ ወኒቆዲሞስ ገነዝዎ ለኢየሱስ በሰንዱናት ለዘተንሥአ እሙታን በመንክር ኪን።(፫ ጊዜ)</t>
+  </si>
+  <si>
+    <t>ሃሌ ሉያ ዮሴፍና ኒቆዲሞስ ድንቅ በሚኾን ጥበብ ከሙታን ተለይቶ የተነሣ ኢየሱስን በበፍታ ገነዙት ።</t>
+  </si>
+  <si>
+    <t>ሃሌ ሉያ ዮሴፍን ኒቆዲሞስን ነዚ ብዘደንቕ ጥበብ ካብ ሙታን ዝተንሥአ ኢየሱስ ብበፍታ ገነዝዎ።</t>
+  </si>
+  <si>
+    <t>Halleluia, Joseph and Nicodemus wrapped with linen cloths Jesus who rose from the dead in wondrous fashion.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  {
+    "meta.date": {
+      "$between": ["$ref:meta.holidays.fasika", "$ref:meta.holidays.paraclete"]
+    }
+  }</t>
   </si>
   <si>
     <t>አንቲ ውእቱ መሶበ ወርቅ ንጹሕ እንተ ውስቴታ መና ኅቡዕ ኅብሰት ዘወረደ እምሰማያት ወሀቤ ሕይወት ለኩሉ ዓለም</t>
@@ -831,6 +850,9 @@
       <c r="I7" s="2" t="s">
         <v>52</v>
       </c>
+      <c r="T7" s="3" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="8">
       <c r="B8" s="3" t="s">
@@ -881,6 +903,9 @@
       </c>
     </row>
     <row r="11">
+      <c r="B11" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="F11" s="2" t="s">
         <v>65</v>
       </c>
@@ -888,86 +913,72 @@
         <v>66</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
+      </c>
+      <c r="T11" s="3" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="12">
-      <c r="B12" s="3" t="s">
+      <c r="F12" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="13">
       <c r="F13" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14">
       <c r="F14" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="M14" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="N14" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="2" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15">
-      <c r="B15" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="F15" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J15" s="3" t="s">
         <v>30</v>
@@ -989,16 +1000,16 @@
         <v>20</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J16" s="3" t="s">
         <v>30</v>
@@ -1020,16 +1031,16 @@
         <v>20</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="J17" s="3" t="s">
         <v>30</v>
@@ -1051,16 +1062,16 @@
         <v>20</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J18" s="3" t="s">
         <v>30</v>
@@ -1082,16 +1093,16 @@
         <v>20</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="J19" s="3" t="s">
         <v>30</v>
@@ -1113,16 +1124,16 @@
         <v>20</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="J20" s="3" t="s">
         <v>30</v>
@@ -1144,16 +1155,16 @@
         <v>20</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J21" s="3" t="s">
         <v>30</v>
@@ -1175,16 +1186,16 @@
         <v>20</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="J22" s="3" t="s">
         <v>30</v>
@@ -1206,16 +1217,16 @@
         <v>20</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="J23" s="3" t="s">
         <v>30</v>
@@ -1237,16 +1248,16 @@
         <v>20</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J24" s="3" t="s">
         <v>30</v>
@@ -1263,11 +1274,36 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" ht="15.75" customHeight="1">
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
+    <row r="25">
+      <c r="B25" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="M25" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="N25" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="O25" s="4"/>
+      <c r="P25" s="4"/>
+      <c r="Q25" s="2" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="F27" s="4"/>
@@ -7058,6 +7094,12 @@
       <c r="G991" s="4"/>
       <c r="H991" s="4"/>
       <c r="I991" s="4"/>
+    </row>
+    <row r="992" ht="15.75" customHeight="1">
+      <c r="F992" s="4"/>
+      <c r="G992" s="4"/>
+      <c r="H992" s="4"/>
+      <c r="I992" s="4"/>
     </row>
   </sheetData>
   <printOptions/>
@@ -7086,48 +7128,48 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -8135,26 +8177,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Gitsawe selection upon date change
</commit_message>
<xml_diff>
--- a/kidase-presentation/samples/Kidase Presentation Template.xlsx
+++ b/kidase-presentation/samples/Kidase Presentation Template.xlsx
@@ -615,19 +615,19 @@
     <t>ተውሳክ</t>
   </si>
   <si>
-    <t>{"meta.ethDate" : {"$eq": "$ref:meta.holidays.timket"}}</t>
+    <t>{"meta.date" : {"$eq": "$ref:meta.holidays.timket"}}</t>
   </si>
   <si>
     <t>ተው2</t>
   </si>
   <si>
-    <t>{"meta.ethDate" : {"$eq": "$ref:meta.holidays.siklet"}}</t>
+    <t>{"meta.date" : {"$eq": "$ref:meta.holidays.siklet"}}</t>
   </si>
   <si>
     <t>ተው3</t>
   </si>
   <si>
-    <t>{"meta.ethDate" : {"$eq": "$ref:meta.holidays.paraclete"}}</t>
+    <t>{"meta.date" : {"$eq": "$ref:meta.holidays.paraclete"}}</t>
   </si>
   <si>
     <t>ሰና1</t>
@@ -636,19 +636,19 @@
     <t>ሰናብት</t>
   </si>
   <si>
-    <t>{"meta.dayOfWeek": {"$eq": "Sun"}, "meta.ethMonthDay": {"$eq": "06-02"}}</t>
+    <t>{"$and": [{"meta.dayOfWeek": {"$eq": "Sun"}}, {"meta.ethMonthDay": {"$eq": "06-01"}}]}</t>
   </si>
   <si>
     <t>ሰና2</t>
   </si>
   <si>
-    <t>{"meta.dayOfWeek": {"$eq": "Sun"}, "meta.ethMonthDay": {"$eq": "06-09"}}</t>
+    <t>{"$and": [{"meta.dayOfWeek": {"$eq": "Sun"}}, {"meta.ethMonthDay": {"$eq": "06-08"}}]}</t>
   </si>
   <si>
     <t>ሰና3</t>
   </si>
   <si>
-    <t>{"meta.dayOfWeek": {"$eq": "Sun"}, "meta.ethMonthDay": {"$eq": "06-16"}}</t>
+    <t>{"$and": [{"meta.dayOfWeek": {"$eq": "Sun"}}, {"meta.ethMonthDay": {"$eq": "06-15"}}]}</t>
   </si>
 </sst>
 </file>
@@ -9560,7 +9560,7 @@
     <col customWidth="1" min="4" max="4" width="24.14"/>
     <col customWidth="1" min="6" max="6" width="19.0"/>
     <col customWidth="1" min="9" max="9" width="25.57"/>
-    <col customWidth="1" min="12" max="12" width="66.29"/>
+    <col customWidth="1" min="12" max="12" width="98.57"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
Optimization on dynamic slide rendering
</commit_message>
<xml_diff>
--- a/kidase-presentation/samples/Kidase Presentation Template.xlsx
+++ b/kidase-presentation/samples/Kidase Presentation Template.xlsx
@@ -568,7 +568,7 @@
     <t>ዘወትር</t>
   </si>
   <si>
-    <t>{"meta.ethMonthDay": {"$eq": "06-03"}}</t>
+    <t>{"meta.ethMonthDay": {"$eq": "06-04"}}</t>
   </si>
   <si>
     <t>ዘወ2</t>
@@ -598,7 +598,7 @@
     <t>ጴጥሮስ</t>
   </si>
   <si>
-    <t>{"meta.ethMonthDay": {"$eq": "06-04"}}</t>
+    <t>{"meta.ethMonthDay": {"$eq": "06-05"}}</t>
   </si>
   <si>
     <t>ዘወ3</t>
@@ -628,7 +628,7 @@
     <t xml:space="preserve">ይሁዳ </t>
   </si>
   <si>
-    <t>{"meta.ethMonthDay": {"$eq": "06-05"}}</t>
+    <t>{"meta.ethMonthDay": {"$eq": "06-06"}}</t>
   </si>
   <si>
     <t>ተው1</t>

</xml_diff>